<commit_message>
Complete files for exceul udemy course
</commit_message>
<xml_diff>
--- a/AutomateSumFunction.xlsx
+++ b/AutomateSumFunction.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/57de5c48f32aaca3/OfficeNewb/Videos/MicrosoftOffice/ExcelVBA/Exercise Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Excel-Udemy\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{030F7A94-F1F0-4339-A243-2D157FBC0326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7620"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EAST RECORDS" sheetId="1" r:id="rId1"/>
@@ -107,7 +108,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
@@ -231,7 +232,7 @@
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal_Sheet1_1" xfId="2"/>
+    <cellStyle name="Normal_Sheet1_1" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -508,23 +509,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:I38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>19</v>
       </c>
@@ -544,7 +545,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -567,7 +568,7 @@
       <c r="H2" s="2"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>0</v>
       </c>
@@ -590,7 +591,7 @@
       <c r="H3" s="2"/>
       <c r="I3" s="3"/>
     </row>
-    <row r="4" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>0</v>
       </c>
@@ -613,7 +614,7 @@
       <c r="H4" s="2"/>
       <c r="I4" s="3"/>
     </row>
-    <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>0</v>
       </c>
@@ -636,7 +637,7 @@
       <c r="H5" s="2"/>
       <c r="I5" s="3"/>
     </row>
-    <row r="6" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
@@ -659,7 +660,7 @@
       <c r="H6" s="2"/>
       <c r="I6" s="3"/>
     </row>
-    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>0</v>
       </c>
@@ -682,7 +683,7 @@
       <c r="H7" s="2"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>0</v>
       </c>
@@ -705,7 +706,7 @@
       <c r="H8" s="2"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>0</v>
       </c>
@@ -728,7 +729,7 @@
       <c r="H9" s="2"/>
       <c r="I9" s="3"/>
     </row>
-    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
@@ -751,7 +752,7 @@
       <c r="H10" s="2"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>0</v>
       </c>
@@ -774,7 +775,7 @@
       <c r="H11" s="2"/>
       <c r="I11" s="3"/>
     </row>
-    <row r="12" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>0</v>
       </c>
@@ -797,7 +798,7 @@
       <c r="H12" s="2"/>
       <c r="I12" s="3"/>
     </row>
-    <row r="13" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>0</v>
       </c>
@@ -820,7 +821,7 @@
       <c r="H13" s="2"/>
       <c r="I13" s="3"/>
     </row>
-    <row r="14" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>0</v>
       </c>
@@ -843,7 +844,7 @@
       <c r="H14" s="2"/>
       <c r="I14" s="3"/>
     </row>
-    <row r="15" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>0</v>
       </c>
@@ -866,118 +867,118 @@
       <c r="H15" s="2"/>
       <c r="I15" s="3"/>
     </row>
-    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F16" s="8"/>
       <c r="G16" s="1"/>
       <c r="H16" s="2"/>
       <c r="I16" s="3"/>
     </row>
-    <row r="17" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G17" s="1"/>
       <c r="H17" s="2"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G18" s="1"/>
       <c r="H18" s="2"/>
       <c r="I18" s="3"/>
     </row>
-    <row r="19" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G19" s="1"/>
       <c r="H19" s="2"/>
       <c r="I19" s="3"/>
     </row>
-    <row r="20" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G20" s="1"/>
       <c r="H20" s="2"/>
       <c r="I20" s="3"/>
     </row>
-    <row r="21" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G21" s="1"/>
       <c r="H21" s="2"/>
       <c r="I21" s="3"/>
     </row>
-    <row r="22" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G22" s="1"/>
       <c r="H22" s="2"/>
       <c r="I22" s="3"/>
     </row>
-    <row r="23" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G23" s="1"/>
       <c r="H23" s="2"/>
       <c r="I23" s="3"/>
     </row>
-    <row r="24" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G24" s="1"/>
       <c r="H24" s="2"/>
       <c r="I24" s="3"/>
     </row>
-    <row r="25" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G25" s="1"/>
       <c r="H25" s="2"/>
       <c r="I25" s="3"/>
     </row>
-    <row r="26" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G26" s="1"/>
       <c r="H26" s="2"/>
       <c r="I26" s="3"/>
     </row>
-    <row r="27" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G27" s="1"/>
       <c r="H27" s="2"/>
       <c r="I27" s="3"/>
     </row>
-    <row r="28" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G28" s="1"/>
       <c r="H28" s="2"/>
       <c r="I28" s="3"/>
     </row>
-    <row r="29" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G29" s="1"/>
       <c r="H29" s="2"/>
       <c r="I29" s="3"/>
     </row>
-    <row r="30" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G30" s="1"/>
       <c r="H30" s="2"/>
       <c r="I30" s="3"/>
     </row>
-    <row r="31" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G31" s="1"/>
       <c r="H31" s="2"/>
       <c r="I31" s="3"/>
     </row>
-    <row r="32" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G32" s="1"/>
       <c r="H32" s="2"/>
       <c r="I32" s="3"/>
     </row>
-    <row r="33" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G33" s="1"/>
       <c r="H33" s="2"/>
       <c r="I33" s="3"/>
     </row>
-    <row r="34" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G34" s="1"/>
       <c r="H34" s="2"/>
       <c r="I34" s="3"/>
     </row>
-    <row r="35" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G35" s="1"/>
       <c r="H35" s="2"/>
       <c r="I35" s="3"/>
     </row>
-    <row r="36" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G36" s="1"/>
       <c r="H36" s="2"/>
       <c r="I36" s="3"/>
     </row>
-    <row r="37" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G37" s="1"/>
       <c r="H37" s="2"/>
       <c r="I37" s="3"/>
     </row>
-    <row r="38" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="7:9" x14ac:dyDescent="0.3">
       <c r="G38" s="1"/>
       <c r="H38" s="2"/>
       <c r="I38" s="3"/>
@@ -988,22 +989,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="17.42578125" customWidth="1"/>
-    <col min="3" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
+    <col min="3" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>19</v>
       </c>
@@ -1023,7 +1024,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6" t="s">
         <v>18</v>
       </c>
@@ -1043,7 +1044,7 @@
         <v>2225</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>18</v>
       </c>
@@ -1063,7 +1064,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6" t="s">
         <v>18</v>
       </c>
@@ -1083,7 +1084,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>18</v>
       </c>
@@ -1103,7 +1104,7 @@
         <v>5700</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="6" t="s">
         <v>18</v>
       </c>
@@ -1123,7 +1124,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
@@ -1143,7 +1144,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>18</v>
       </c>
@@ -1163,7 +1164,7 @@
         <v>3785</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>11250</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
         <v>18</v>
       </c>
@@ -1203,7 +1204,7 @@
         <v>14345</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>18</v>
       </c>
@@ -1223,7 +1224,7 @@
         <v>15000</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>18</v>
       </c>
@@ -1243,7 +1244,7 @@
         <v>16085</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>18</v>
       </c>
@@ -1263,7 +1264,7 @@
         <v>31250</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>18</v>
       </c>
@@ -1283,7 +1284,7 @@
         <v>43500</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>18</v>
       </c>
@@ -1303,7 +1304,7 @@
         <v>212000</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>18</v>
       </c>
@@ -1323,7 +1324,7 @@
         <v>75000</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F17" s="8"/>
     </row>
   </sheetData>
@@ -1332,23 +1333,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" customWidth="1"/>
-    <col min="3" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="1" max="1" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>19</v>
       </c>
@@ -1368,7 +1369,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>15</v>
       </c>
@@ -1388,7 +1389,7 @@
         <v>2500</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>15</v>
       </c>
@@ -1408,7 +1409,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
@@ -1428,7 +1429,7 @@
         <v>2710</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>15</v>
       </c>
@@ -1448,7 +1449,7 @@
         <v>2780</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>15</v>
       </c>
@@ -1468,7 +1469,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>15</v>
       </c>
@@ -1488,7 +1489,7 @@
         <v>3805</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>15</v>
       </c>
@@ -1508,7 +1509,7 @@
         <v>6650</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>15</v>
       </c>
@@ -1528,7 +1529,7 @@
         <v>10710</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>15</v>
       </c>
@@ -1548,7 +1549,7 @@
         <v>14300</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>15</v>
       </c>
@@ -1568,7 +1569,7 @@
         <v>19755</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>15</v>
       </c>
@@ -1588,7 +1589,7 @@
         <v>18060</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>15</v>
       </c>
@@ -1608,7 +1609,7 @@
         <v>35740</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
@@ -1628,7 +1629,7 @@
         <v>41550</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>15</v>
       </c>
@@ -1648,7 +1649,7 @@
         <v>76830</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F16" s="8"/>
     </row>
   </sheetData>
@@ -1657,7 +1658,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
@@ -1665,15 +1666,15 @@
       <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>19</v>
       </c>
@@ -1693,7 +1694,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
@@ -1713,7 +1714,7 @@
         <v>6450</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>16</v>
       </c>
@@ -1733,7 +1734,7 @@
         <v>1685</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
@@ -1753,7 +1754,7 @@
         <v>2200</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>16</v>
       </c>
@@ -1773,7 +1774,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1793,7 +1794,7 @@
         <v>2425</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>16</v>
       </c>
@@ -1813,7 +1814,7 @@
         <v>3750</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>16</v>
       </c>
@@ -1833,7 +1834,7 @@
         <v>8670</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>16</v>
       </c>
@@ -1853,7 +1854,7 @@
         <v>39400</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>16</v>
       </c>
@@ -1873,7 +1874,7 @@
         <v>14100</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="6" t="s">
         <v>16</v>
       </c>
@@ -1893,7 +1894,7 @@
         <v>15750</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
         <v>16</v>
       </c>
@@ -1913,7 +1914,7 @@
         <v>19665</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
@@ -1933,7 +1934,7 @@
         <v>34250</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>16</v>
       </c>
@@ -1953,7 +1954,7 @@
         <v>72500</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>16</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>180570</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>16</v>
       </c>
@@ -1993,7 +1994,7 @@
         <v>74940</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
       <c r="F17" s="8"/>
     </row>
   </sheetData>

</xml_diff>